<commit_message>
R10 version 3.0 data. deff_p estimated from the initial design weights as 1 / prob.
</commit_message>
<xml_diff>
--- a/tables/variables-2.xlsx
+++ b/tables/variables-2.xlsx
@@ -807,7 +807,7 @@
         <v>12.778</v>
       </c>
       <c r="N2" t="n">
-        <v>12.631</v>
+        <v>12.664</v>
       </c>
       <c r="O2" t="n">
         <v>0.991</v>
@@ -819,7 +819,7 @@
         <v>0.986</v>
       </c>
       <c r="R2" t="n">
-        <v>0.958</v>
+        <v>0.955</v>
       </c>
     </row>
     <row r="3">
@@ -863,7 +863,7 @@
         <v>0.326</v>
       </c>
       <c r="N3" t="n">
-        <v>0.446</v>
+        <v>0.439</v>
       </c>
       <c r="O3" t="n">
         <v>0.103</v>
@@ -919,7 +919,7 @@
         <v>2.553</v>
       </c>
       <c r="N4" t="n">
-        <v>2.569</v>
+        <v>2.59</v>
       </c>
       <c r="O4" t="n">
         <v>0.997</v>
@@ -931,7 +931,7 @@
         <v>0.997</v>
       </c>
       <c r="R4" t="n">
-        <v>0.989</v>
+        <v>0.988</v>
       </c>
     </row>
     <row r="5">
@@ -975,7 +975,7 @@
         <v>4.661</v>
       </c>
       <c r="N5" t="n">
-        <v>4.901</v>
+        <v>4.968</v>
       </c>
       <c r="O5" t="n">
         <v>0.268</v>
@@ -987,7 +987,7 @@
         <v>0.261</v>
       </c>
       <c r="R5" t="n">
-        <v>0.236</v>
+        <v>0.245</v>
       </c>
     </row>
     <row r="6">
@@ -1031,7 +1031,7 @@
         <v>700.749</v>
       </c>
       <c r="N6" t="n">
-        <v>594.219</v>
+        <v>600.767</v>
       </c>
       <c r="O6" t="n">
         <v>0.355</v>
@@ -1043,7 +1043,7 @@
         <v>0.349</v>
       </c>
       <c r="R6" t="n">
-        <v>0.296</v>
+        <v>0.299</v>
       </c>
     </row>
     <row r="7">
@@ -1087,7 +1087,7 @@
         <v>30.168</v>
       </c>
       <c r="N7" t="n">
-        <v>27.019</v>
+        <v>26.695</v>
       </c>
       <c r="O7" t="n">
         <v>0.848</v>
@@ -1099,7 +1099,7 @@
         <v>0.801</v>
       </c>
       <c r="R7" t="n">
-        <v>0.717</v>
+        <v>0.716</v>
       </c>
     </row>
     <row r="8">
@@ -1143,7 +1143,7 @@
         <v>33.574</v>
       </c>
       <c r="N8" t="n">
-        <v>31.941</v>
+        <v>31.803</v>
       </c>
       <c r="O8" t="n">
         <v>0.872</v>
@@ -1155,7 +1155,7 @@
         <v>0.841</v>
       </c>
       <c r="R8" t="n">
-        <v>0.809</v>
+        <v>0.812</v>
       </c>
     </row>
     <row r="9">
@@ -1199,7 +1199,7 @@
         <v>13.12</v>
       </c>
       <c r="N9" t="n">
-        <v>13.151</v>
+        <v>13.069</v>
       </c>
       <c r="O9" t="n">
         <v>0.347</v>
@@ -1211,7 +1211,7 @@
         <v>0.33</v>
       </c>
       <c r="R9" t="n">
-        <v>0.332</v>
+        <v>0.331</v>
       </c>
     </row>
     <row r="10">
@@ -1255,7 +1255,7 @@
         <v>1958.581</v>
       </c>
       <c r="N10" t="n">
-        <v>1929.119</v>
+        <v>1926.614</v>
       </c>
       <c r="O10" t="n">
         <v>0.998</v>
@@ -1267,7 +1267,7 @@
         <v>0.996</v>
       </c>
       <c r="R10" t="n">
-        <v>0.979</v>
+        <v>0.978</v>
       </c>
     </row>
     <row r="11">
@@ -1311,7 +1311,7 @@
         <v>1.907</v>
       </c>
       <c r="N11" t="n">
-        <v>1.982</v>
+        <v>1.979</v>
       </c>
       <c r="O11" t="n">
         <v>0.99</v>
@@ -1367,7 +1367,7 @@
         <v>4.85</v>
       </c>
       <c r="N12" t="n">
-        <v>5.227</v>
+        <v>5.203</v>
       </c>
       <c r="O12" t="n">
         <v>0.912</v>
@@ -1379,7 +1379,7 @@
         <v>0.922</v>
       </c>
       <c r="R12" t="n">
-        <v>0.943</v>
+        <v>0.942</v>
       </c>
     </row>
     <row r="13">
@@ -1423,7 +1423,7 @@
         <v>2.089</v>
       </c>
       <c r="N13" t="n">
-        <v>2.038</v>
+        <v>2.021</v>
       </c>
       <c r="O13" t="n">
         <v>0.971</v>
@@ -1479,7 +1479,7 @@
         <v>2.063</v>
       </c>
       <c r="N14" t="n">
-        <v>2.096</v>
+        <v>2.094</v>
       </c>
       <c r="O14" t="n">
         <v>0.982</v>
@@ -1491,7 +1491,7 @@
         <v>0.981</v>
       </c>
       <c r="R14" t="n">
-        <v>0.984</v>
+        <v>0.985</v>
       </c>
     </row>
     <row r="15">
@@ -1535,7 +1535,7 @@
         <v>7.391</v>
       </c>
       <c r="N15" t="n">
-        <v>7.077</v>
+        <v>7.093</v>
       </c>
       <c r="O15" t="n">
         <v>0.996</v>
@@ -1591,7 +1591,7 @@
         <v>2.205</v>
       </c>
       <c r="N16" t="n">
-        <v>2.203</v>
+        <v>2.187</v>
       </c>
       <c r="O16" t="n">
         <v>0.999</v>
@@ -1603,7 +1603,7 @@
         <v>0.999</v>
       </c>
       <c r="R16" t="n">
-        <v>0.996</v>
+        <v>0.995</v>
       </c>
     </row>
     <row r="17">
@@ -1647,7 +1647,7 @@
         <v>4.965</v>
       </c>
       <c r="N17" t="n">
-        <v>5.2</v>
+        <v>5.264</v>
       </c>
       <c r="O17" t="n">
         <v>0.965</v>
@@ -1659,7 +1659,7 @@
         <v>0.958</v>
       </c>
       <c r="R17" t="n">
-        <v>0.973</v>
+        <v>0.974</v>
       </c>
     </row>
     <row r="18">
@@ -1703,7 +1703,7 @@
         <v>5.208</v>
       </c>
       <c r="N18" t="n">
-        <v>5.366</v>
+        <v>5.438</v>
       </c>
       <c r="O18" t="n">
         <v>0.966</v>
@@ -1759,7 +1759,7 @@
         <v>4.834</v>
       </c>
       <c r="N19" t="n">
-        <v>4.935</v>
+        <v>5.025</v>
       </c>
       <c r="O19" t="n">
         <v>0.962</v>
@@ -1771,7 +1771,7 @@
         <v>0.957</v>
       </c>
       <c r="R19" t="n">
-        <v>0.97</v>
+        <v>0.971</v>
       </c>
     </row>
     <row r="20">
@@ -1815,7 +1815,7 @@
         <v>3.725</v>
       </c>
       <c r="N20" t="n">
-        <v>3.833</v>
+        <v>3.895</v>
       </c>
       <c r="O20" t="n">
         <v>0.906</v>
@@ -1827,7 +1827,7 @@
         <v>0.899</v>
       </c>
       <c r="R20" t="n">
-        <v>0.866</v>
+        <v>0.868</v>
       </c>
     </row>
     <row r="21">
@@ -1871,7 +1871,7 @@
         <v>4.292</v>
       </c>
       <c r="N21" t="n">
-        <v>4.397</v>
+        <v>4.441</v>
       </c>
       <c r="O21" t="n">
         <v>0.892</v>
@@ -1883,7 +1883,7 @@
         <v>0.854</v>
       </c>
       <c r="R21" t="n">
-        <v>0.884</v>
+        <v>0.888</v>
       </c>
     </row>
     <row r="22">
@@ -1927,7 +1927,7 @@
         <v>2.656</v>
       </c>
       <c r="N22" t="n">
-        <v>2.605</v>
+        <v>2.595</v>
       </c>
       <c r="O22" t="n">
         <v>0.997</v>
@@ -1983,7 +1983,7 @@
         <v>5.59</v>
       </c>
       <c r="N23" t="n">
-        <v>5.436</v>
+        <v>5.487</v>
       </c>
       <c r="O23" t="n">
         <v>0.993</v>
@@ -2039,7 +2039,7 @@
         <v>4.962</v>
       </c>
       <c r="N24" t="n">
-        <v>4.742</v>
+        <v>4.825</v>
       </c>
       <c r="O24" t="n">
         <v>0.996</v>
@@ -2095,7 +2095,7 @@
         <v>5.047</v>
       </c>
       <c r="N25" t="n">
-        <v>4.743</v>
+        <v>4.773</v>
       </c>
       <c r="O25" t="n">
         <v>0.998</v>
@@ -2151,7 +2151,7 @@
         <v>4.496</v>
       </c>
       <c r="N26" t="n">
-        <v>4.391</v>
+        <v>4.375</v>
       </c>
       <c r="O26" t="n">
         <v>0.993</v>
@@ -2163,7 +2163,7 @@
         <v>0.99</v>
       </c>
       <c r="R26" t="n">
-        <v>0.984</v>
+        <v>0.985</v>
       </c>
     </row>
     <row r="27">
@@ -2207,7 +2207,7 @@
         <v>5.066</v>
       </c>
       <c r="N27" t="n">
-        <v>5.177</v>
+        <v>5.162</v>
       </c>
       <c r="O27" t="n">
         <v>0.971</v>
@@ -2263,7 +2263,7 @@
         <v>5.128</v>
       </c>
       <c r="N28" t="n">
-        <v>4.804</v>
+        <v>4.762</v>
       </c>
       <c r="O28" t="n">
         <v>0.984</v>
@@ -2275,7 +2275,7 @@
         <v>0.975</v>
       </c>
       <c r="R28" t="n">
-        <v>0.981</v>
+        <v>0.982</v>
       </c>
     </row>
     <row r="29">
@@ -2319,7 +2319,7 @@
         <v>5.596</v>
       </c>
       <c r="N29" t="n">
-        <v>4.967</v>
+        <v>5.003</v>
       </c>
       <c r="O29" t="n">
         <v>0.958</v>
@@ -2331,7 +2331,7 @@
         <v>0.962</v>
       </c>
       <c r="R29" t="n">
-        <v>0.963</v>
+        <v>0.964</v>
       </c>
     </row>
     <row r="30">
@@ -2375,7 +2375,7 @@
         <v>4.307</v>
       </c>
       <c r="N30" t="n">
-        <v>4.282</v>
+        <v>4.274</v>
       </c>
       <c r="O30" t="n">
         <v>0.971</v>
@@ -2387,7 +2387,7 @@
         <v>0.965</v>
       </c>
       <c r="R30" t="n">
-        <v>0.978</v>
+        <v>0.979</v>
       </c>
     </row>
     <row r="31">
@@ -2431,7 +2431,7 @@
         <v>5.5</v>
       </c>
       <c r="N31" t="n">
-        <v>5.447</v>
+        <v>5.449</v>
       </c>
       <c r="O31" t="n">
         <v>0.993</v>
@@ -2487,7 +2487,7 @@
         <v>7.074</v>
       </c>
       <c r="N32" t="n">
-        <v>6.923</v>
+        <v>6.932</v>
       </c>
       <c r="O32" t="n">
         <v>0.997</v>
@@ -2499,7 +2499,7 @@
         <v>0.995</v>
       </c>
       <c r="R32" t="n">
-        <v>0.99</v>
+        <v>0.991</v>
       </c>
     </row>
     <row r="33">
@@ -2543,7 +2543,7 @@
         <v>4.154</v>
       </c>
       <c r="N33" t="n">
-        <v>4.302</v>
+        <v>4.283</v>
       </c>
       <c r="O33" t="n">
         <v>0.918</v>
@@ -2599,7 +2599,7 @@
         <v>5.226</v>
       </c>
       <c r="N34" t="n">
-        <v>5.158</v>
+        <v>5.162</v>
       </c>
       <c r="O34" t="n">
         <v>0.981</v>
@@ -2655,7 +2655,7 @@
         <v>6.371</v>
       </c>
       <c r="N35" t="n">
-        <v>6.259</v>
+        <v>6.21</v>
       </c>
       <c r="O35" t="n">
         <v>0.993</v>
@@ -2667,7 +2667,7 @@
         <v>0.993</v>
       </c>
       <c r="R35" t="n">
-        <v>0.991</v>
+        <v>0.992</v>
       </c>
     </row>
     <row r="36">
@@ -2711,7 +2711,7 @@
         <v>3.59</v>
       </c>
       <c r="N36" t="n">
-        <v>3.452</v>
+        <v>3.436</v>
       </c>
       <c r="O36" t="n">
         <v>0.987</v>
@@ -2767,7 +2767,7 @@
         <v>4.419</v>
       </c>
       <c r="N37" t="n">
-        <v>4.471</v>
+        <v>4.433</v>
       </c>
       <c r="O37" t="n">
         <v>0.98</v>
@@ -2779,7 +2779,7 @@
         <v>0.977</v>
       </c>
       <c r="R37" t="n">
-        <v>0.983</v>
+        <v>0.982</v>
       </c>
     </row>
     <row r="38">
@@ -2823,7 +2823,7 @@
         <v>3.534</v>
       </c>
       <c r="N38" t="n">
-        <v>3.424</v>
+        <v>3.41</v>
       </c>
       <c r="O38" t="n">
         <v>0.982</v>
@@ -2879,7 +2879,7 @@
         <v>4.708</v>
       </c>
       <c r="N39" t="n">
-        <v>4.704</v>
+        <v>4.681</v>
       </c>
       <c r="O39" t="n">
         <v>0.92</v>
@@ -2935,7 +2935,7 @@
         <v>5.429</v>
       </c>
       <c r="N40" t="n">
-        <v>5.36</v>
+        <v>5.405</v>
       </c>
       <c r="O40" t="n">
         <v>0.911</v>
@@ -2947,7 +2947,7 @@
         <v>0.904</v>
       </c>
       <c r="R40" t="n">
-        <v>0.871</v>
+        <v>0.872</v>
       </c>
     </row>
     <row r="41">
@@ -2991,7 +2991,7 @@
         <v>0.277</v>
       </c>
       <c r="N41" t="n">
-        <v>0.26</v>
+        <v>0.269</v>
       </c>
       <c r="O41" t="n">
         <v>0.994</v>
@@ -3003,7 +3003,7 @@
         <v>0.996</v>
       </c>
       <c r="R41" t="n">
-        <v>0.973</v>
+        <v>0.972</v>
       </c>
     </row>
     <row r="42">
@@ -3047,7 +3047,7 @@
         <v>0.902</v>
       </c>
       <c r="N42" t="n">
-        <v>0.915</v>
+        <v>0.907</v>
       </c>
       <c r="O42" t="n">
         <v>1</v>
@@ -3059,7 +3059,7 @@
         <v>0.999</v>
       </c>
       <c r="R42" t="n">
-        <v>0.996</v>
+        <v>0.995</v>
       </c>
     </row>
     <row r="43">
@@ -3103,7 +3103,7 @@
         <v>0.345</v>
       </c>
       <c r="N43" t="n">
-        <v>0.316</v>
+        <v>0.312</v>
       </c>
       <c r="O43" t="n">
         <v>0.638</v>
@@ -3115,7 +3115,7 @@
         <v>0.648</v>
       </c>
       <c r="R43" t="n">
-        <v>0.649</v>
+        <v>0.645</v>
       </c>
     </row>
     <row r="44">
@@ -3159,7 +3159,7 @@
         <v>0.465</v>
       </c>
       <c r="N44" t="n">
-        <v>0.452</v>
+        <v>0.448</v>
       </c>
       <c r="O44" t="n">
         <v>0.979</v>
@@ -3171,7 +3171,7 @@
         <v>0.973</v>
       </c>
       <c r="R44" t="n">
-        <v>0.974</v>
+        <v>0.975</v>
       </c>
     </row>
     <row r="45">
@@ -3215,7 +3215,7 @@
         <v>0.133</v>
       </c>
       <c r="N45" t="n">
-        <v>0.104</v>
+        <v>0.106</v>
       </c>
       <c r="O45" t="n">
         <v>0.997</v>
@@ -3227,7 +3227,7 @@
         <v>0.996</v>
       </c>
       <c r="R45" t="n">
-        <v>0.993</v>
+        <v>0.992</v>
       </c>
     </row>
     <row r="46">
@@ -3327,7 +3327,7 @@
         <v>0.952</v>
       </c>
       <c r="N47" t="n">
-        <v>0.95</v>
+        <v>0.947</v>
       </c>
       <c r="O47" t="n">
         <v>0.999</v>
@@ -3551,7 +3551,7 @@
         <v>0.009</v>
       </c>
       <c r="N51" t="n">
-        <v>0.011</v>
+        <v>0.012</v>
       </c>
       <c r="O51" t="n">
         <v>1</v>
@@ -3607,7 +3607,7 @@
         <v>0.01</v>
       </c>
       <c r="N52" t="n">
-        <v>0.018</v>
+        <v>0.019</v>
       </c>
       <c r="O52" t="n">
         <v>1</v>
@@ -3663,7 +3663,7 @@
         <v>0.075</v>
       </c>
       <c r="N53" t="n">
-        <v>0.087</v>
+        <v>0.095</v>
       </c>
       <c r="O53" t="n">
         <v>0.991</v>
@@ -3719,7 +3719,7 @@
         <v>0.007</v>
       </c>
       <c r="N54" t="n">
-        <v>0.011</v>
+        <v>0.014</v>
       </c>
       <c r="O54" t="n">
         <v>1</v>
@@ -3831,7 +3831,7 @@
         <v>0.925</v>
       </c>
       <c r="N56" t="n">
-        <v>0.911</v>
+        <v>0.903</v>
       </c>
       <c r="O56" t="n">
         <v>1</v>
@@ -3887,7 +3887,7 @@
         <v>0.015</v>
       </c>
       <c r="N57" t="n">
-        <v>0.019</v>
+        <v>0.022</v>
       </c>
       <c r="O57" t="n">
         <v>1</v>
@@ -3943,7 +3943,7 @@
         <v>0.019</v>
       </c>
       <c r="N58" t="n">
-        <v>0.018</v>
+        <v>0.019</v>
       </c>
       <c r="O58" t="n">
         <v>1</v>
@@ -3999,7 +3999,7 @@
         <v>0.009</v>
       </c>
       <c r="N59" t="n">
-        <v>0.012</v>
+        <v>0.014</v>
       </c>
       <c r="O59" t="n">
         <v>1</v>
@@ -4055,7 +4055,7 @@
         <v>0.001</v>
       </c>
       <c r="N60" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="O60" t="n">
         <v>1</v>
@@ -4111,7 +4111,7 @@
         <v>0.013</v>
       </c>
       <c r="N61" t="n">
-        <v>0.015</v>
+        <v>0.019</v>
       </c>
       <c r="O61" t="n">
         <v>1</v>
@@ -4167,7 +4167,7 @@
         <v>0.005</v>
       </c>
       <c r="N62" t="n">
-        <v>0.01</v>
+        <v>0.011</v>
       </c>
       <c r="O62" t="n">
         <v>1</v>
@@ -4223,7 +4223,7 @@
         <v>0.156</v>
       </c>
       <c r="N63" t="n">
-        <v>0.148</v>
+        <v>0.15</v>
       </c>
       <c r="O63" t="n">
         <v>0.993</v>
@@ -4235,7 +4235,7 @@
         <v>0.996</v>
       </c>
       <c r="R63" t="n">
-        <v>0.978</v>
+        <v>0.977</v>
       </c>
     </row>
     <row r="64">
@@ -4279,7 +4279,7 @@
         <v>0.79</v>
       </c>
       <c r="N64" t="n">
-        <v>0.756</v>
+        <v>0.757</v>
       </c>
       <c r="O64" t="n">
         <v>0.917</v>
@@ -4291,7 +4291,7 @@
         <v>0.908</v>
       </c>
       <c r="R64" t="n">
-        <v>0.876</v>
+        <v>0.877</v>
       </c>
     </row>
     <row r="65">
@@ -4335,7 +4335,7 @@
         <v>0.86</v>
       </c>
       <c r="N65" t="n">
-        <v>0.874</v>
+        <v>0.86</v>
       </c>
       <c r="O65" t="n">
         <v>0.994</v>
@@ -4391,7 +4391,7 @@
         <v>0.465</v>
       </c>
       <c r="N66" t="n">
-        <v>0.468</v>
+        <v>0.466</v>
       </c>
       <c r="O66" t="n">
         <v>0.999</v>
@@ -4403,7 +4403,7 @@
         <v>1</v>
       </c>
       <c r="R66" t="n">
-        <v>0.99</v>
+        <v>0.989</v>
       </c>
     </row>
     <row r="67">
@@ -4447,7 +4447,7 @@
         <v>0.358</v>
       </c>
       <c r="N67" t="n">
-        <v>0.296</v>
+        <v>0.294</v>
       </c>
       <c r="O67" t="n">
         <v>0.868</v>
@@ -4459,7 +4459,7 @@
         <v>0.89</v>
       </c>
       <c r="R67" t="n">
-        <v>0.863</v>
+        <v>0.854</v>
       </c>
     </row>
     <row r="68">
@@ -4503,7 +4503,7 @@
         <v>0.867</v>
       </c>
       <c r="N68" t="n">
-        <v>0.878</v>
+        <v>0.865</v>
       </c>
       <c r="O68" t="n">
         <v>0.998</v>
@@ -4515,7 +4515,7 @@
         <v>0.998</v>
       </c>
       <c r="R68" t="n">
-        <v>0.992</v>
+        <v>0.991</v>
       </c>
     </row>
     <row r="69">
@@ -4559,7 +4559,7 @@
         <v>0.354</v>
       </c>
       <c r="N69" t="n">
-        <v>0.312</v>
+        <v>0.315</v>
       </c>
       <c r="O69" t="n">
         <v>0.455</v>
@@ -4615,7 +4615,7 @@
         <v>0.595</v>
       </c>
       <c r="N70" t="n">
-        <v>0.624</v>
+        <v>0.611</v>
       </c>
       <c r="O70" t="n">
         <v>0.996</v>
@@ -4627,7 +4627,7 @@
         <v>0.993</v>
       </c>
       <c r="R70" t="n">
-        <v>0.991</v>
+        <v>0.992</v>
       </c>
     </row>
     <row r="71">
@@ -4671,7 +4671,7 @@
         <v>0.105</v>
       </c>
       <c r="N71" t="n">
-        <v>0.074</v>
+        <v>0.086</v>
       </c>
       <c r="O71" t="n">
         <v>0.422</v>
@@ -4683,7 +4683,7 @@
         <v>0.399</v>
       </c>
       <c r="R71" t="n">
-        <v>0.37</v>
+        <v>0.383</v>
       </c>
     </row>
     <row r="72">
@@ -4727,7 +4727,7 @@
         <v>#NUM!</v>
       </c>
       <c r="N72" t="n">
-        <v>0.535</v>
+        <v>0.538</v>
       </c>
       <c r="O72" t="e">
         <v>#NUM!</v>
@@ -4739,7 +4739,7 @@
         <v>#NUM!</v>
       </c>
       <c r="R72" t="n">
-        <v>0.982</v>
+        <v>0.981</v>
       </c>
     </row>
     <row r="73">
@@ -4783,7 +4783,7 @@
         <v>0.134</v>
       </c>
       <c r="N73" t="n">
-        <v>0.13</v>
+        <v>0.127</v>
       </c>
       <c r="O73" t="n">
         <v>0.281</v>
@@ -4795,7 +4795,7 @@
         <v>0.285</v>
       </c>
       <c r="R73" t="n">
-        <v>0.272</v>
+        <v>0.271</v>
       </c>
     </row>
     <row r="74">
@@ -4839,7 +4839,7 @@
         <v>0.287</v>
       </c>
       <c r="N74" t="n">
-        <v>0.274</v>
+        <v>0.273</v>
       </c>
       <c r="O74" t="n">
         <v>0.996</v>
@@ -4851,7 +4851,7 @@
         <v>0.994</v>
       </c>
       <c r="R74" t="n">
-        <v>0.972</v>
+        <v>0.971</v>
       </c>
     </row>
     <row r="75">
@@ -4895,7 +4895,7 @@
         <v>0.12</v>
       </c>
       <c r="N75" t="n">
-        <v>0.112</v>
+        <v>0.111</v>
       </c>
       <c r="O75" t="n">
         <v>0.281</v>
@@ -4907,7 +4907,7 @@
         <v>0.285</v>
       </c>
       <c r="R75" t="n">
-        <v>0.272</v>
+        <v>0.27</v>
       </c>
     </row>
     <row r="76">
@@ -4963,7 +4963,7 @@
         <v>0.988</v>
       </c>
       <c r="R76" t="n">
-        <v>0.987</v>
+        <v>0.988</v>
       </c>
     </row>
     <row r="77">
@@ -5007,7 +5007,7 @@
         <v>0.065</v>
       </c>
       <c r="N77" t="n">
-        <v>0.056</v>
+        <v>0.057</v>
       </c>
       <c r="O77" t="n">
         <v>0.918</v>
@@ -5019,7 +5019,7 @@
         <v>0.914</v>
       </c>
       <c r="R77" t="n">
-        <v>0.877</v>
+        <v>0.878</v>
       </c>
     </row>
   </sheetData>

</xml_diff>